<commit_message>
performance comparison graphs integrated in documentation
</commit_message>
<xml_diff>
--- a/results/diffusion_results.xlsx
+++ b/results/diffusion_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="36960" windowHeight="15340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="raw Measurements" sheetId="4" r:id="rId1"/>
@@ -989,11 +989,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>3D</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> Diffusion, 1 Core Westmere Xeon CPU </a:t>
+              <a:t>3D Diffusion, 1 Core Westmere Xeon CPU </a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1001,7 +997,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
+              <a:rPr lang="de-DE"/>
               <a:t>[Millions of Stencils per Second]</a:t>
             </a:r>
           </a:p>
@@ -1166,16 +1162,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="-2132046040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1204,6 +1190,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1237,11 +1233,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>3D Diffusion,</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> 6 Core Westmere Xeon CPU (1 Socket)</a:t>
+              <a:t>3D Diffusion, 6 Core Westmere Xeon CPU (1 Socket)</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -1249,7 +1241,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
+              <a:rPr lang="de-DE"/>
               <a:t> [Millions of Stencils per Second]</a:t>
             </a:r>
           </a:p>
@@ -1455,16 +1447,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="-2131826680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1493,6 +1475,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1533,11 +1525,7 @@
             </a:br>
             <a:r>
               <a:rPr lang="de-DE"/>
-              <a:t>[</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t>Millions of Stencils per Second]</a:t>
+              <a:t>[Millions of Stencils per Second]</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1717,16 +1705,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="-2131867864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1755,6 +1733,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1787,21 +1775,15 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
+              <a:rPr lang="de-DE"/>
               <a:t>Speedup 3D Diffusion</a:t>
             </a:r>
             <a:br>
-              <a:rPr lang="de-DE" baseline="0"/>
+              <a:rPr lang="de-DE"/>
             </a:br>
             <a:r>
-              <a:rPr lang="de-DE" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>1x NVIDIA Kepler K20x </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="de-DE" baseline="0"/>
-              <a:t>vs. Portable C on 6 Core Westmere (1 Socket) </a:t>
+              <a:rPr lang="de-DE"/>
+              <a:t>1x NVIDIA Kepler K20x vs. Portable C on 6 Core Westmere (1 Socket) </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1975,16 +1957,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400"/>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="-2130253720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -2013,6 +1985,16 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1800"/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -3543,8 +3525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J131" sqref="J131"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="I161" sqref="I161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>